<commit_message>
Actualizar dependencias y agregar página 8_Proyectados.py
</commit_message>
<xml_diff>
--- a/Desembolsos_Acumulados.xlsx
+++ b/Desembolsos_Acumulados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERSONAL\Downloads\desembolsos-main\desembolsos-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D56988C-CA6B-4E6C-B39E-EEA94099CE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783E540D-6729-439F-9357-61ADDB90165E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-1275" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -713,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="R38" sqref="R38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>